<commit_message>
Include total virtualization overhead during network I/O
modified:   cpu_network_io_performance.xlsx
</commit_message>
<xml_diff>
--- a/haas/temp/cpu_network_io_performance.xlsx
+++ b/haas/temp/cpu_network_io_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Downloads/pci-passthrough/haas/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D6760D-9F87-554C-92E9-0449A80FFE87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193BD99D-26CE-674A-A500-18DF1BE423F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11840" yWindow="880" windowWidth="16380" windowHeight="13860" xr2:uid="{7EF91B35-F92D-604F-AA73-432BB79FBB5E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="86">
   <si>
     <t>Baremetal</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>CASE D in HOST</t>
+  </si>
+  <si>
+    <t>NETWORK VIRTUALIZATION CPU OVERHEAD</t>
+  </si>
+  <si>
+    <t>TOTAL VIRTAUALIZATION CPU OVERHEAD</t>
   </si>
 </sst>
 </file>
@@ -637,11 +643,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D12BE3-462E-3F4C-8DBA-1D6977DE4EF9}">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -930,7 +934,15 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -961,8 +973,38 @@
       <c r="J19" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -993,8 +1035,38 @@
       <c r="J20">
         <v>122.38</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20">
+        <v>5.7</v>
+      </c>
+      <c r="N20">
+        <v>5.7</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>68.25</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>3.69</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>222.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1025,8 +1097,38 @@
       <c r="J21">
         <v>46.96</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21">
+        <v>68.61</v>
+      </c>
+      <c r="N21">
+        <v>68.64</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>50.7</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>33.659999999999997</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>146.91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1057,8 +1159,38 @@
       <c r="J24" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1089,8 +1221,38 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25">
+        <v>194.04</v>
+      </c>
+      <c r="N25">
+        <v>194.07</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>3.09</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>2.91</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>99.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1121,8 +1283,38 @@
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26">
+        <v>125.28</v>
+      </c>
+      <c r="N26">
+        <v>125.31</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>43.65</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>31.08</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>99.96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1153,8 +1345,38 @@
       <c r="J29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1185,8 +1407,38 @@
       <c r="J30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30">
+        <v>199.83</v>
+      </c>
+      <c r="N30">
+        <v>199.89</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0.24</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>99.87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1217,8 +1469,38 @@
       <c r="J31">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>30</v>
+      </c>
+      <c r="M31">
+        <v>199.74</v>
+      </c>
+      <c r="N31">
+        <v>199.77</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0.24</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1249,8 +1531,38 @@
       <c r="J34" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1281,8 +1593,38 @@
       <c r="J35">
         <v>196.34</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>29</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0.02</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0.86</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>2.78</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>196.34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1313,8 +1655,38 @@
       <c r="J36">
         <v>117.64</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0.66</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>41.42</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>117.64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -1325,7 +1697,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1336,7 +1708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1347,7 +1719,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -1358,7 +1730,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1369,7 +1741,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1380,7 +1752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -1391,7 +1763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Update the CPU and Network I/O performance
The host saturates the network bandwidth (37.39 Gbps) with the
Mellanox ConnectX-3.

modified:   cpu_network_io_performance.xlsx
</commit_message>
<xml_diff>
--- a/haas/temp/cpu_network_io_performance.xlsx
+++ b/haas/temp/cpu_network_io_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Downloads/pci-passthrough/haas/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193BD99D-26CE-674A-A500-18DF1BE423F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38AA837-893B-2E47-9509-C83B6780AAD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="880" windowWidth="16380" windowHeight="13860" xr2:uid="{7EF91B35-F92D-604F-AA73-432BB79FBB5E}"/>
+    <workbookView xWindow="11840" yWindow="880" windowWidth="16380" windowHeight="13860" activeTab="1" xr2:uid="{7EF91B35-F92D-604F-AA73-432BB79FBB5E}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="87">
   <si>
     <t>Baremetal</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>TOTAL VIRTAUALIZATION CPU OVERHEAD</t>
+  </si>
+  <si>
+    <t>37.39|0.08</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D12BE3-462E-3F4C-8DBA-1D6977DE4EF9}">
   <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1762,6 +1767,9 @@
       <c r="C47" t="s">
         <v>46</v>
       </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2157,7 +2165,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790D54A8-3F75-044D-AD19-558761BB2381}">
   <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4111,6 +4121,9 @@
       <c r="C96" t="s">
         <v>46</v>
       </c>
+      <c r="D96" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">

</xml_diff>

<commit_message>
Update CPU utilization and DID efficiency data
modified:   cpu_network_io_performance.xlsx
modified:   did_efficiency.xlsx
</commit_message>
<xml_diff>
--- a/haas/temp/cpu_network_io_performance.xlsx
+++ b/haas/temp/cpu_network_io_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Downloads/pci-passthrough/haas/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38AA837-893B-2E47-9509-C83B6780AAD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F870F851-5661-7C4E-BC53-4EDA42CCC80E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11840" yWindow="880" windowWidth="16380" windowHeight="13860" activeTab="1" xr2:uid="{7EF91B35-F92D-604F-AA73-432BB79FBB5E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="100">
   <si>
     <t>Baremetal</t>
   </si>
@@ -171,9 +171,6 @@
     <t>934.21|1.66</t>
   </si>
   <si>
-    <t>37.07|0.22</t>
-  </si>
-  <si>
     <t>934.67|5.93</t>
   </si>
   <si>
@@ -292,6 +289,48 @@
   </si>
   <si>
     <t>37.39|0.08</t>
+  </si>
+  <si>
+    <t>CASE C</t>
+  </si>
+  <si>
+    <t>redo using the ping flood</t>
+  </si>
+  <si>
+    <t>0.29|0.03</t>
+  </si>
+  <si>
+    <t>ENABLE HLT EXITING</t>
+  </si>
+  <si>
+    <t>SYSTEM</t>
+  </si>
+  <si>
+    <t>vHOST</t>
+  </si>
+  <si>
+    <t>VFIO</t>
+  </si>
+  <si>
+    <t>DISABLE HLT EXITING</t>
+  </si>
+  <si>
+    <t>934.27|1.97</t>
+  </si>
+  <si>
+    <t>37.45|0.08</t>
+  </si>
+  <si>
+    <t>IN GUEST</t>
+  </si>
+  <si>
+    <t>e1000e</t>
+  </si>
+  <si>
+    <t>mellanox</t>
+  </si>
+  <si>
+    <t>CASE C in HOST</t>
   </si>
 </sst>
 </file>
@@ -646,13 +685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D12BE3-462E-3F4C-8DBA-1D6977DE4EF9}">
-  <dimension ref="A1:U85"/>
+  <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -941,10 +980,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="L18" t="s">
         <v>84</v>
-      </c>
-      <c r="L18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1321,7 +1360,7 @@
     </row>
     <row r="29" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>20</v>
@@ -1351,7 +1390,7 @@
         <v>28</v>
       </c>
       <c r="L29" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>20</v>
@@ -1386,16 +1425,16 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>199.84</v>
+        <v>4.34</v>
       </c>
       <c r="C30">
-        <v>199.84</v>
+        <v>4.34</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.16</v>
+        <v>93.06</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1410,22 +1449,22 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>102.6</v>
       </c>
       <c r="L30" t="s">
         <v>29</v>
       </c>
       <c r="M30">
-        <v>199.83</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="N30">
-        <v>199.89</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30">
-        <v>0.24</v>
+        <v>93.06</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -1440,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <v>99.87</v>
+        <v>202.59</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
@@ -1448,16 +1487,16 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>199.76</v>
+        <v>90.48</v>
       </c>
       <c r="C31">
-        <v>199.76</v>
+        <v>90.48</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0.24</v>
+        <v>85.08</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1472,22 +1511,22 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>24.44</v>
       </c>
       <c r="L31" t="s">
         <v>30</v>
       </c>
       <c r="M31">
-        <v>199.74</v>
+        <v>90.48</v>
       </c>
       <c r="N31">
-        <v>199.77</v>
+        <v>90.51</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
-        <v>0.24</v>
+        <v>85.14</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -1502,12 +1541,12 @@
         <v>0</v>
       </c>
       <c r="U31">
-        <v>99.99</v>
+        <v>124.35</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>20</v>
@@ -1537,7 +1576,7 @@
         <v>28</v>
       </c>
       <c r="L34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>20</v>
@@ -1572,22 +1611,22 @@
         <v>29</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>199.84</v>
       </c>
       <c r="C35">
-        <v>0.02</v>
+        <v>199.84</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0.86</v>
+        <v>0.16</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1596,28 +1635,28 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>196.34</v>
+        <v>0</v>
       </c>
       <c r="L35" t="s">
         <v>29</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>199.83</v>
       </c>
       <c r="N35">
-        <v>0.02</v>
+        <v>199.89</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
       <c r="P35">
-        <v>0.86</v>
+        <v>0.24</v>
       </c>
       <c r="Q35">
         <v>0</v>
       </c>
       <c r="R35">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="S35">
         <v>0</v>
@@ -1626,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="U35">
-        <v>196.34</v>
+        <v>99.87</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
@@ -1634,22 +1673,22 @@
         <v>30</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>199.76</v>
       </c>
       <c r="C36">
-        <v>0.66</v>
+        <v>199.76</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>40.299999999999997</v>
+        <v>0.24</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36">
-        <v>41.42</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1658,28 +1697,28 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>117.64</v>
+        <v>0</v>
       </c>
       <c r="L36" t="s">
         <v>30</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>199.74</v>
       </c>
       <c r="N36">
-        <v>0.66</v>
+        <v>199.77</v>
       </c>
       <c r="O36">
         <v>0</v>
       </c>
       <c r="P36">
-        <v>40.299999999999997</v>
+        <v>0.24</v>
       </c>
       <c r="Q36">
         <v>0</v>
       </c>
       <c r="R36">
-        <v>41.42</v>
+        <v>0</v>
       </c>
       <c r="S36">
         <v>0</v>
@@ -1688,471 +1727,937 @@
         <v>0</v>
       </c>
       <c r="U36">
-        <v>117.64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0.02</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.86</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>2.78</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>196.34</v>
+      </c>
+      <c r="L40" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0.02</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0.86</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>2.78</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>196.34</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0.66</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>41.42</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>117.64</v>
+      </c>
+      <c r="L41" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0.66</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>41.42</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>117.64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47" t="s">
-        <v>86</v>
+        <v>41</v>
+      </c>
+      <c r="G47" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="G48" t="s">
+        <v>89</v>
+      </c>
+      <c r="H48" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" t="s">
+        <v>90</v>
+      </c>
+      <c r="K48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" t="s">
+        <v>91</v>
+      </c>
+      <c r="H49">
+        <v>5.7</v>
+      </c>
+      <c r="I49">
+        <v>5.7</v>
+      </c>
+      <c r="J49">
+        <v>71.94</v>
+      </c>
+      <c r="K49">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="I50">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="J50">
+        <v>93.06</v>
+      </c>
+      <c r="K50">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>31</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
         <v>47</v>
       </c>
-      <c r="C48" t="s">
+      <c r="G53" t="s">
+        <v>93</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>90</v>
+      </c>
+      <c r="K53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C54" t="s">
         <v>49</v>
       </c>
-      <c r="C49" t="s">
+      <c r="F54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>91</v>
+      </c>
+      <c r="H54">
+        <v>194.04</v>
+      </c>
+      <c r="I54">
+        <v>194.07</v>
+      </c>
+      <c r="J54">
+        <v>6</v>
+      </c>
+      <c r="K54">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55">
+        <v>199.83</v>
+      </c>
+      <c r="I55">
+        <v>199.89</v>
+      </c>
+      <c r="J55">
+        <v>0.24</v>
+      </c>
+      <c r="K55">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C56" t="s">
         <v>51</v>
       </c>
-      <c r="C50" t="s">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" t="s">
+        <v>20</v>
+      </c>
+      <c r="I57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" t="s">
+        <v>90</v>
+      </c>
+      <c r="K57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0.06</v>
+      </c>
+      <c r="J58">
+        <v>9.1</v>
+      </c>
+      <c r="K58">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" t="s">
+        <v>96</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0.02</v>
+      </c>
+      <c r="J59">
+        <v>3.64</v>
+      </c>
+      <c r="K59">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B60">
+        <v>120634</v>
+      </c>
+      <c r="C60">
+        <v>3304283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>54</v>
       </c>
-      <c r="B54">
-        <v>120634</v>
-      </c>
-      <c r="C54">
-        <v>3304283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B61">
+        <v>569</v>
+      </c>
+      <c r="C61">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>55</v>
       </c>
-      <c r="B55">
-        <v>569</v>
-      </c>
-      <c r="C55">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B62">
+        <v>2464</v>
+      </c>
+      <c r="C62">
+        <v>942143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>56</v>
       </c>
-      <c r="B56">
-        <v>2464</v>
-      </c>
-      <c r="C56">
-        <v>942143</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B63">
+        <v>267682</v>
+      </c>
+      <c r="C63">
+        <v>261691</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>57</v>
       </c>
-      <c r="B57">
-        <v>267682</v>
-      </c>
-      <c r="C57">
-        <v>261691</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B64">
+        <v>1110</v>
+      </c>
+      <c r="C64">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>58</v>
       </c>
-      <c r="B58">
-        <v>1110</v>
-      </c>
-      <c r="C58">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59">
+      <c r="B65">
         <v>120</v>
       </c>
-      <c r="C59">
+      <c r="C65">
         <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60">
-        <v>42748</v>
-      </c>
-      <c r="C60">
-        <v>134874</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61">
-        <v>169</v>
-      </c>
-      <c r="C61">
-        <v>75945</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62">
-        <v>2040</v>
-      </c>
-      <c r="C62">
-        <v>16361</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63">
-        <v>1037</v>
-      </c>
-      <c r="C63">
-        <v>24348</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64">
-        <f>SUM(B54:B63)</f>
-        <v>438573</v>
-      </c>
-      <c r="C64">
-        <f>SUM(C54:C63)</f>
-        <v>4760860</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>32</v>
-      </c>
-      <c r="B66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66" t="s">
-        <v>30</v>
+        <v>59</v>
+      </c>
+      <c r="B66">
+        <v>42748</v>
+      </c>
+      <c r="C66">
+        <v>134874</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B67">
-        <v>117271</v>
+        <v>169</v>
       </c>
       <c r="C67">
-        <v>3151062</v>
+        <v>75945</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B68">
-        <v>954</v>
+        <v>2040</v>
       </c>
       <c r="C68">
-        <v>4349</v>
+        <v>16361</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B69">
-        <v>344564</v>
+        <v>1037</v>
       </c>
       <c r="C69">
-        <v>1188715</v>
+        <v>24348</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B70">
-        <v>1110</v>
+        <f>SUM(B60:B69)</f>
+        <v>438573</v>
       </c>
       <c r="C70">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71">
-        <v>120</v>
-      </c>
-      <c r="C71">
-        <v>120</v>
+        <f>SUM(C60:C69)</f>
+        <v>4760860</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>60</v>
-      </c>
-      <c r="B72">
-        <v>42087</v>
-      </c>
-      <c r="C72">
-        <v>124407</v>
+        <v>32</v>
+      </c>
+      <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B73">
-        <v>117</v>
+        <v>117271</v>
       </c>
       <c r="C73">
-        <v>415</v>
+        <v>3151062</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B74">
-        <v>1413</v>
+        <v>954</v>
       </c>
       <c r="C74">
-        <v>8505</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B75">
-        <v>36052</v>
+        <v>344564</v>
       </c>
       <c r="C75">
-        <v>36098</v>
+        <v>1188715</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B76">
-        <f>SUM(B67:B75)</f>
-        <v>543688</v>
+        <v>1110</v>
       </c>
       <c r="C76">
-        <f>SUM(C67:C75)</f>
-        <v>4514744</v>
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77">
+        <v>120</v>
+      </c>
+      <c r="C77">
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>33</v>
-      </c>
-      <c r="B78" t="s">
-        <v>29</v>
-      </c>
-      <c r="C78" t="s">
-        <v>30</v>
+        <v>59</v>
+      </c>
+      <c r="B78">
+        <v>42087</v>
+      </c>
+      <c r="C78">
+        <v>124407</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>415</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B80">
-        <v>29887</v>
+        <v>1413</v>
       </c>
       <c r="C80">
-        <v>29881</v>
+        <v>8505</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B81">
-        <v>1110</v>
+        <v>36052</v>
       </c>
       <c r="C81">
-        <v>1073</v>
+        <v>36098</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B82">
-        <v>120</v>
+        <f>SUM(B73:B81)</f>
+        <v>543688</v>
       </c>
       <c r="C82">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>60</v>
-      </c>
-      <c r="B83">
-        <v>51298</v>
-      </c>
-      <c r="C83">
-        <v>269695</v>
+        <f>SUM(C73:C81)</f>
+        <v>4514744</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>63</v>
-      </c>
-      <c r="B84">
-        <v>36024</v>
-      </c>
-      <c r="C84">
-        <v>36063</v>
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B85">
-        <f>SUM(B79:B84)</f>
+        <v>323792</v>
+      </c>
+      <c r="C85">
+        <v>4785929</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>55</v>
+      </c>
+      <c r="B86">
+        <v>645</v>
+      </c>
+      <c r="C86">
+        <v>13114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87">
+        <v>1110</v>
+      </c>
+      <c r="C87">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88">
+        <v>119</v>
+      </c>
+      <c r="C88">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89">
+        <v>51259</v>
+      </c>
+      <c r="C89">
+        <v>235121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90">
+        <v>100</v>
+      </c>
+      <c r="C90">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>62</v>
+      </c>
+      <c r="B91">
+        <v>724</v>
+      </c>
+      <c r="C91">
+        <v>16260</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92">
+        <f>SUM(B85:B91)</f>
+        <v>377749</v>
+      </c>
+      <c r="C92">
+        <f>SUM(C85:C91)</f>
+        <v>5051677</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>33</v>
+      </c>
+      <c r="B94" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>55</v>
+      </c>
+      <c r="B96">
+        <v>29887</v>
+      </c>
+      <c r="C96">
+        <v>29881</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>57</v>
+      </c>
+      <c r="B97">
+        <v>1110</v>
+      </c>
+      <c r="C97">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>58</v>
+      </c>
+      <c r="B98">
+        <v>120</v>
+      </c>
+      <c r="C98">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B99">
+        <v>51298</v>
+      </c>
+      <c r="C99">
+        <v>269695</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>62</v>
+      </c>
+      <c r="B100">
+        <v>36024</v>
+      </c>
+      <c r="C100">
+        <v>36063</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>63</v>
+      </c>
+      <c r="B101">
+        <f>SUM(B95:B100)</f>
         <v>118440</v>
       </c>
-      <c r="C85">
-        <f>SUM(C79:C84)</f>
+      <c r="C101">
+        <f>SUM(C95:C100)</f>
         <v>336832</v>
       </c>
     </row>
@@ -2163,10 +2668,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790D54A8-3F75-044D-AD19-558761BB2381}">
-  <dimension ref="A1:K134"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2224,42 +2729,42 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2294,7 +2799,7 @@
         <v>99.933000000000007</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2329,7 +2834,7 @@
         <v>92.957999999999998</v>
       </c>
       <c r="K7" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -2364,47 +2869,47 @@
         <v>97.882999999999996</v>
       </c>
       <c r="K8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -2439,7 +2944,7 @@
         <v>99.933000000000007</v>
       </c>
       <c r="K13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2474,7 +2979,7 @@
         <v>62.317</v>
       </c>
       <c r="K14" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2509,7 +3014,7 @@
         <v>56.082999999999998</v>
       </c>
       <c r="K15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -2632,72 +3137,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -2732,7 +3214,7 @@
         <v>99.983000000000004</v>
       </c>
       <c r="K29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -2767,7 +3249,7 @@
         <v>25.882999999999999</v>
       </c>
       <c r="K30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2802,7 +3284,7 @@
         <v>96.5</v>
       </c>
       <c r="K31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -2837,47 +3319,47 @@
         <v>99.941999999999993</v>
       </c>
       <c r="K32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -2912,7 +3394,7 @@
         <v>99.957999999999998</v>
       </c>
       <c r="K36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -2947,7 +3429,7 @@
         <v>3.05</v>
       </c>
       <c r="K37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2982,7 +3464,7 @@
         <v>43.908000000000001</v>
       </c>
       <c r="K38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -3017,52 +3499,52 @@
         <v>99.95</v>
       </c>
       <c r="K39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -3097,7 +3579,7 @@
         <v>99.933000000000007</v>
       </c>
       <c r="K45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -3132,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -3167,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="K47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -3202,47 +3684,47 @@
         <v>99.95</v>
       </c>
       <c r="K48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -3277,7 +3759,7 @@
         <v>99.95</v>
       </c>
       <c r="K52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -3312,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="K53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -3347,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="K54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3382,52 +3864,52 @@
         <v>99.95</v>
       </c>
       <c r="K55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="I60" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3435,13 +3917,13 @@
         <v>0</v>
       </c>
       <c r="B61">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>8.3000000000000004E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -3459,10 +3941,10 @@
         <v>0</v>
       </c>
       <c r="J61">
-        <v>99.867000000000004</v>
+        <v>99.98</v>
       </c>
       <c r="K61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3470,13 +3952,13 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>99.908000000000001</v>
+        <v>2.9</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>9.1999999999999998E-2</v>
+        <v>92.77</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -3488,16 +3970,16 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>99.917000000000002</v>
+        <v>2.9</v>
       </c>
       <c r="I62">
         <v>0</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>4.33</v>
       </c>
       <c r="K62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -3505,13 +3987,13 @@
         <v>2</v>
       </c>
       <c r="B63">
-        <v>99.924999999999997</v>
+        <v>1.44</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>7.4999999999999997E-2</v>
+        <v>0.3</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -3523,16 +4005,16 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <v>99.924999999999997</v>
+        <v>1.44</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>0</v>
+        <v>98.26</v>
       </c>
       <c r="K63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -3540,13 +4022,13 @@
         <v>3</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -3564,64 +4046,99 @@
         <v>0</v>
       </c>
       <c r="J64">
-        <v>99.974999999999994</v>
+        <v>99.95</v>
       </c>
       <c r="K64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="H67" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="I67" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I68" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K68" s="1" t="s">
-        <v>76</v>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>0.03</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0.06</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>99.92</v>
+      </c>
+      <c r="K68" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>47.66</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>8.0000000000000002E-3</v>
+        <v>52.34</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -3633,30 +4150,30 @@
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>47.65</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69">
-        <v>99.992000000000004</v>
+        <v>0</v>
       </c>
       <c r="K69" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B70">
-        <v>99.766999999999996</v>
+        <v>42.83</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>0.23300000000000001</v>
+        <v>32.729999999999997</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -3668,30 +4185,30 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>99.757999999999996</v>
+        <v>42.83</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
       <c r="J70">
-        <v>0</v>
+        <v>24.44</v>
       </c>
       <c r="K70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B71">
-        <v>99.992000000000004</v>
+        <v>0.03</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>8.0000000000000002E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -3703,96 +4220,61 @@
         <v>0</v>
       </c>
       <c r="H71">
-        <v>99.992000000000004</v>
+        <v>0</v>
       </c>
       <c r="I71">
         <v>0</v>
       </c>
       <c r="J71">
-        <v>0</v>
+        <v>99.96</v>
       </c>
       <c r="K71" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>3</v>
-      </c>
-      <c r="B72">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-      <c r="D72">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="J72">
-        <v>99.933000000000007</v>
-      </c>
-      <c r="K72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="K76" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3800,19 +4282,19 @@
         <v>0</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>2.7829999999999999</v>
+        <v>0</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3824,10 +4306,10 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>97.216999999999999</v>
+        <v>99.867000000000004</v>
       </c>
       <c r="K77" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -3835,13 +4317,13 @@
         <v>1</v>
       </c>
       <c r="B78">
-        <v>1.7000000000000001E-2</v>
+        <v>99.908000000000001</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>0.86699999999999999</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -3853,16 +4335,16 @@
         <v>0</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>99.917000000000002</v>
       </c>
       <c r="I78">
         <v>0</v>
       </c>
       <c r="J78">
-        <v>99.117000000000004</v>
+        <v>0</v>
       </c>
       <c r="K78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -3870,13 +4352,13 @@
         <v>2</v>
       </c>
       <c r="B79">
-        <v>1.7000000000000001E-2</v>
+        <v>99.924999999999997</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>2.5000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -3888,625 +4370,1110 @@
         <v>0</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>99.924999999999997</v>
       </c>
       <c r="I79">
         <v>0</v>
       </c>
       <c r="J79">
-        <v>99.957999999999998</v>
+        <v>0</v>
       </c>
       <c r="K79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>99.974999999999994</v>
+      </c>
+      <c r="K80" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>65</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="H84" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="I84" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I82" s="1" t="s">
+      <c r="J84" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J82" s="1" t="s">
+      <c r="K84" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K82" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>0</v>
-      </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>41.417000000000002</v>
-      </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
-      </c>
-      <c r="I83">
-        <v>0</v>
-      </c>
-      <c r="J83">
-        <v>58.582999999999998</v>
-      </c>
-      <c r="K83" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>1</v>
-      </c>
-      <c r="B84">
-        <v>0.65</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84">
-        <v>0</v>
-      </c>
-      <c r="J84">
-        <v>59.05</v>
-      </c>
-      <c r="K84" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>99.992000000000004</v>
+      </c>
+      <c r="K85" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>99.766999999999996</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>99.757999999999996</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87">
         <v>2</v>
       </c>
-      <c r="B85">
+      <c r="B87">
+        <v>99.992000000000004</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-      <c r="D85">
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>99.992000000000004</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="F85">
-        <v>0</v>
-      </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85">
-        <v>0</v>
-      </c>
-      <c r="J85">
-        <v>99.95</v>
-      </c>
-      <c r="K85" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>35</v>
-      </c>
-      <c r="B88" t="s">
-        <v>29</v>
-      </c>
-      <c r="C88" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>19</v>
-      </c>
-      <c r="B89" t="s">
-        <v>36</v>
-      </c>
-      <c r="C89" t="s">
-        <v>37</v>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>99.933000000000007</v>
+      </c>
+      <c r="K88" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>31</v>
-      </c>
-      <c r="B90" t="s">
-        <v>38</v>
-      </c>
-      <c r="C90" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>2.7829999999999999</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>97.216999999999999</v>
+      </c>
+      <c r="K93" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>99.117000000000004</v>
+      </c>
+      <c r="K94" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="B95">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>99.957999999999998</v>
+      </c>
+      <c r="K95" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>65</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>41.417000000000002</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>58.582999999999998</v>
+      </c>
+      <c r="K99" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>0.65</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>59.05</v>
+      </c>
+      <c r="K100" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>99.95</v>
+      </c>
+      <c r="K101" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>32</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B107" t="s">
         <v>40</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C107" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>86</v>
+      </c>
+      <c r="B108" t="s">
+        <v>88</v>
+      </c>
+      <c r="C108" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>33</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B109" t="s">
         <v>42</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C109" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>44</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B111" t="s">
         <v>29</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C111" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>19</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B112" t="s">
         <v>45</v>
       </c>
-      <c r="C96" t="s">
-        <v>46</v>
-      </c>
-      <c r="D96" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>31</v>
-      </c>
-      <c r="B97" t="s">
-        <v>47</v>
-      </c>
-      <c r="C97" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>32</v>
-      </c>
-      <c r="B98" t="s">
-        <v>49</v>
-      </c>
-      <c r="C98" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>33</v>
-      </c>
-      <c r="B99" t="s">
-        <v>51</v>
-      </c>
-      <c r="C99" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>53</v>
-      </c>
-      <c r="B102" t="s">
-        <v>29</v>
-      </c>
-      <c r="C102" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>54</v>
-      </c>
-      <c r="B103">
-        <v>120634</v>
-      </c>
-      <c r="C103">
-        <v>3304283</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>55</v>
-      </c>
-      <c r="B104">
-        <v>569</v>
-      </c>
-      <c r="C104">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>56</v>
-      </c>
-      <c r="B105">
-        <v>2464</v>
-      </c>
-      <c r="C105">
-        <v>942143</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>57</v>
-      </c>
-      <c r="B106">
-        <v>267682</v>
-      </c>
-      <c r="C106">
-        <v>261691</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>58</v>
-      </c>
-      <c r="B107">
-        <v>1110</v>
-      </c>
-      <c r="C107">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B108">
-        <v>120</v>
-      </c>
-      <c r="C108">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>60</v>
-      </c>
-      <c r="B109">
-        <v>42748</v>
-      </c>
-      <c r="C109">
-        <v>134874</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>61</v>
-      </c>
-      <c r="B110">
-        <v>169</v>
-      </c>
-      <c r="C110">
-        <v>75945</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>62</v>
-      </c>
-      <c r="B111">
-        <v>2040</v>
-      </c>
-      <c r="C111">
-        <v>16361</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>63</v>
-      </c>
-      <c r="B112">
-        <v>1037</v>
-      </c>
-      <c r="C112">
-        <v>24348</v>
+      <c r="C112" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>64</v>
-      </c>
-      <c r="B113">
-        <f>SUM(B103:B112)</f>
-        <v>438573</v>
-      </c>
-      <c r="C113">
-        <f>SUM(C103:C112)</f>
-        <v>4760860</v>
+        <v>31</v>
+      </c>
+      <c r="B113" t="s">
+        <v>46</v>
+      </c>
+      <c r="C113" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="B115" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="C115" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>54</v>
-      </c>
-      <c r="B116">
-        <v>117271</v>
-      </c>
-      <c r="C116">
-        <v>3151062</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>55</v>
-      </c>
-      <c r="B117">
-        <v>954</v>
-      </c>
-      <c r="C117">
-        <v>4349</v>
+        <v>33</v>
+      </c>
+      <c r="B116" t="s">
+        <v>50</v>
+      </c>
+      <c r="C116" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>56</v>
-      </c>
-      <c r="B118">
-        <v>344564</v>
-      </c>
-      <c r="C118">
-        <v>1188715</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>58</v>
-      </c>
-      <c r="B119">
-        <v>1110</v>
-      </c>
-      <c r="C119">
-        <v>1073</v>
+        <v>52</v>
+      </c>
+      <c r="B119" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B120">
-        <v>120</v>
+        <v>120634</v>
       </c>
       <c r="C120">
-        <v>120</v>
+        <v>3304283</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B121">
-        <v>42087</v>
+        <v>569</v>
       </c>
       <c r="C121">
-        <v>124407</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B122">
-        <v>117</v>
+        <v>2464</v>
       </c>
       <c r="C122">
-        <v>415</v>
+        <v>942143</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B123">
-        <v>1413</v>
+        <v>267682</v>
       </c>
       <c r="C123">
-        <v>8505</v>
+        <v>261691</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B124">
-        <v>36052</v>
+        <v>1110</v>
       </c>
       <c r="C124">
-        <v>36098</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B125">
-        <f>SUM(B116:B124)</f>
-        <v>543688</v>
+        <v>120</v>
       </c>
       <c r="C125">
-        <f>SUM(C116:C124)</f>
-        <v>4514744</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>59</v>
+      </c>
+      <c r="B126">
+        <v>42748</v>
+      </c>
+      <c r="C126">
+        <v>134874</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>33</v>
-      </c>
-      <c r="B127" t="s">
-        <v>29</v>
-      </c>
-      <c r="C127" t="s">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="B127">
+        <v>169</v>
+      </c>
+      <c r="C127">
+        <v>75945</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>2040</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>16361</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B129">
-        <v>29887</v>
+        <v>1037</v>
       </c>
       <c r="C129">
-        <v>29881</v>
+        <v>24348</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B130">
-        <v>1110</v>
+        <f>SUM(B120:B129)</f>
+        <v>438573</v>
       </c>
       <c r="C130">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>59</v>
-      </c>
-      <c r="B131">
-        <v>120</v>
-      </c>
-      <c r="C131">
-        <v>120</v>
+        <f>SUM(C120:C129)</f>
+        <v>4760860</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>60</v>
-      </c>
-      <c r="B132">
-        <v>51298</v>
-      </c>
-      <c r="C132">
-        <v>269695</v>
+        <v>32</v>
+      </c>
+      <c r="B132" t="s">
+        <v>29</v>
+      </c>
+      <c r="C132" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B133">
-        <v>36024</v>
+        <v>117271</v>
       </c>
       <c r="C133">
-        <v>36063</v>
+        <v>3151062</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B134">
-        <f>SUM(B128:B133)</f>
+        <v>954</v>
+      </c>
+      <c r="C134">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>55</v>
+      </c>
+      <c r="B135">
+        <v>344564</v>
+      </c>
+      <c r="C135">
+        <v>1188715</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>57</v>
+      </c>
+      <c r="B136">
+        <v>1110</v>
+      </c>
+      <c r="C136">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>58</v>
+      </c>
+      <c r="B137">
+        <v>120</v>
+      </c>
+      <c r="C137">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>59</v>
+      </c>
+      <c r="B138">
+        <v>42087</v>
+      </c>
+      <c r="C138">
+        <v>124407</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>60</v>
+      </c>
+      <c r="B139">
+        <v>117</v>
+      </c>
+      <c r="C139">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>61</v>
+      </c>
+      <c r="B140">
+        <v>1413</v>
+      </c>
+      <c r="C140">
+        <v>8505</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>62</v>
+      </c>
+      <c r="B141">
+        <v>36052</v>
+      </c>
+      <c r="C141">
+        <v>36098</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>63</v>
+      </c>
+      <c r="B142">
+        <f>SUM(B133:B141)</f>
+        <v>543688</v>
+      </c>
+      <c r="C142">
+        <f>SUM(C133:C141)</f>
+        <v>4514744</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144" t="s">
+        <v>29</v>
+      </c>
+      <c r="C144" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>56</v>
+      </c>
+      <c r="B145">
+        <v>323792</v>
+      </c>
+      <c r="C145">
+        <v>4785929</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>55</v>
+      </c>
+      <c r="B146">
+        <v>645</v>
+      </c>
+      <c r="C146">
+        <v>13114</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>57</v>
+      </c>
+      <c r="B147">
+        <v>1110</v>
+      </c>
+      <c r="C147">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>58</v>
+      </c>
+      <c r="B148">
+        <v>119</v>
+      </c>
+      <c r="C148">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>59</v>
+      </c>
+      <c r="B149">
+        <v>51259</v>
+      </c>
+      <c r="C149">
+        <v>235121</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>60</v>
+      </c>
+      <c r="B150">
+        <v>100</v>
+      </c>
+      <c r="C150">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>62</v>
+      </c>
+      <c r="B151">
+        <v>724</v>
+      </c>
+      <c r="C151">
+        <v>16260</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>63</v>
+      </c>
+      <c r="B152">
+        <f>SUM(B145:B151)</f>
+        <v>377749</v>
+      </c>
+      <c r="C152">
+        <f>SUM(C145:C151)</f>
+        <v>5051677</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>33</v>
+      </c>
+      <c r="B154" t="s">
+        <v>29</v>
+      </c>
+      <c r="C154" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>53</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>55</v>
+      </c>
+      <c r="B156">
+        <v>29887</v>
+      </c>
+      <c r="C156">
+        <v>29881</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>57</v>
+      </c>
+      <c r="B157">
+        <v>1110</v>
+      </c>
+      <c r="C157">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>58</v>
+      </c>
+      <c r="B158">
+        <v>120</v>
+      </c>
+      <c r="C158">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>59</v>
+      </c>
+      <c r="B159">
+        <v>51298</v>
+      </c>
+      <c r="C159">
+        <v>269695</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>62</v>
+      </c>
+      <c r="B160">
+        <v>36024</v>
+      </c>
+      <c r="C160">
+        <v>36063</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>63</v>
+      </c>
+      <c r="B161">
+        <f>SUM(B155:B160)</f>
         <v>118440</v>
       </c>
-      <c r="C134">
-        <f>SUM(C128:C133)</f>
+      <c r="C161">
+        <f>SUM(C155:C160)</f>
         <v>336832</v>
       </c>
     </row>

</xml_diff>